<commit_message>
Add new validation rules for property consistency checks
- Implement rules 708, 716, 717, 676, and 725 in the SQL validation script.
- Each rule addresses specific conditions related to address structure, name length, NPN coherence, and required complements in units.
- Create corresponding tables for each rule to store validation results.
- Update the consolidated Excel file to include the new validation rules.
</commit_message>
<xml_diff>
--- a/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
+++ b/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erikka Lopez\Desktop\validaciones\IgacValidaciones\validar_consistencia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A697C9EA-1C85-4E15-AF08-9FB7C9BF3EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264B503B-770C-46BB-904E-A3137DEBC615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="850">
   <si>
     <t>id</t>
   </si>
@@ -3036,6 +3036,24 @@
   </si>
   <si>
     <t>Todos los registros son No_Estructurada</t>
+  </si>
+  <si>
+    <t>Todos los registros cumplen</t>
+  </si>
+  <si>
+    <t>No tenemos ILC_DatosAdicionalesLevantamientoCatastral</t>
+  </si>
+  <si>
+    <t>No tenemos info en complemento</t>
+  </si>
+  <si>
+    <t>No hay PH Matriz en nuestros datos</t>
+  </si>
+  <si>
+    <t>No tenemos ilc_predio_informalidad</t>
+  </si>
+  <si>
+    <t>No tenemos ILC_TramitesDerechosTerritoriales</t>
   </si>
 </sst>
 </file>
@@ -3059,7 +3077,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3081,12 +3099,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3118,7 +3130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3169,15 +3181,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3484,9 +3487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H225"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4465,210 +4468,210 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="18">
+      <c r="A38" s="10">
         <v>713</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="H38" s="20">
+      <c r="H38" s="12">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="18">
+      <c r="A39" s="10">
         <v>714</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="H39" s="20">
+      <c r="H39" s="12">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="18">
+      <c r="A40" s="10">
         <v>715</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="H40" s="20">
+      <c r="H40" s="12">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="6">
+      <c r="A41" s="11">
         <v>716</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="11">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="6">
+      <c r="A42" s="10">
         <v>717</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="12">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A43" s="6">
+      <c r="A43" s="10">
         <v>718</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="12">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="6">
+      <c r="A44" s="16">
         <v>719</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H44" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A45" s="6">
+      <c r="A45" s="16">
         <v>720</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="G45" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
@@ -4698,211 +4701,211 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A47" s="6">
+    <row r="47" spans="1:8" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="16">
         <v>721</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G47" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A48" s="6">
+      <c r="A48" s="16">
         <v>722</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="G48" s="7" t="s">
+      <c r="G48" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="6">
+      <c r="A49" s="16">
         <v>723</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G49" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="H49" s="8">
+      <c r="H49" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A50" s="6">
+      <c r="A50" s="16">
         <v>724</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="G50" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H50" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="6">
+      <c r="A51" s="10">
         <v>725</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="G51" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="H51" s="8">
+      <c r="H51" s="12">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A52" s="6">
+      <c r="A52" s="16">
         <v>726</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="G52" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H52" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="6">
+      <c r="A53" s="16">
         <v>727</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G53" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="6">
+      <c r="A54" s="16">
         <v>728</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G54" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="17">
         <v>45815.481844355723</v>
       </c>
     </row>
@@ -9003,10 +9006,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72DF236-5369-47CC-87A0-4923FC7C346E}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9550,6 +9553,202 @@
       <c r="B40" s="5" t="s">
         <v>164</v>
       </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>716</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>717</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="4">
+        <v>254827</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>718</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>719</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>720</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>676</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>721</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>722</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>723</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>724</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>725</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>726</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>727</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>728</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>849</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new validation rule 680 for property consistency checks
- Implement rule 680 in the SQL validation script, focusing on NPN validation for Condominio.Unidad_Predial.
- Create a corresponding table to store validation results for this rule.
- Remove temporary Excel file and update the existing consolidated Excel file to reflect the changes.
</commit_message>
<xml_diff>
--- a/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
+++ b/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erikka Lopez\Desktop\validaciones\IgacValidaciones\validar_consistencia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39B8661-AE73-4901-A648-A828C99030CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F25DF4-1BA5-47EF-B49A-3DDF0B6A96F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3496,9 +3496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H225"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4997,28 +4997,28 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A58" s="6">
+      <c r="A58" s="10">
         <v>680</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F58" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="G58" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="H58" s="8">
+      <c r="H58" s="12">
         <v>45815.481844355723</v>
       </c>
     </row>
@@ -9017,8 +9017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72DF236-5369-47CC-87A0-4923FC7C346E}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9805,6 +9805,9 @@
       <c r="B58" s="5" t="s">
         <v>234</v>
       </c>
+      <c r="C58" s="4">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new validation rule 779 for property consistency checks
- Implement rule 779 in the SQL validation script, focusing on properties designated as institutional, cultural, educational, or religious without associated construction units.
- Create a corresponding table to store validation results for this rule.
- Update the consolidated Excel file to reflect the addition of the new validation rule.
</commit_message>
<xml_diff>
--- a/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
+++ b/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erikka Lopez\Desktop\validaciones\IgacValidaciones\validar_consistencia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13426FD3-FF9E-4029-84A9-FE844FAE8BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D73BA71-173E-4ED3-8CC5-833D3A4C2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3120,7 +3120,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3157,12 +3157,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3191,7 +3185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3257,15 +3251,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3573,8 +3558,8 @@
   <dimension ref="A1:H225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G100" sqref="G100"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6163,54 +6148,54 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A100" s="23">
+      <c r="A100" s="10">
         <v>778</v>
       </c>
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C100" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="D100" s="24" t="s">
+      <c r="D100" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="E100" s="24" t="s">
+      <c r="E100" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="F100" s="24" t="s">
+      <c r="F100" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="G100" s="24" t="s">
+      <c r="G100" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="H100" s="25">
+      <c r="H100" s="12">
         <v>45815.481990740744</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A101" s="6">
+      <c r="A101" s="10">
         <v>779</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B101" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C101" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="E101" s="7" t="s">
+      <c r="E101" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="F101" s="7" t="s">
+      <c r="F101" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="G101" s="7" t="s">
+      <c r="G101" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="H101" s="8">
+      <c r="H101" s="12">
         <v>45815.481991131652</v>
       </c>
     </row>
@@ -9187,8 +9172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72DF236-5369-47CC-87A0-4923FC7C346E}">
   <dimension ref="A1:D236"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10522,15 +10507,27 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B100" s="5" t="e">
+      <c r="A100" s="4">
+        <v>778</v>
+      </c>
+      <c r="B100" s="5" t="str">
         <f>VLOOKUP(A100,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
+        <v>Los predios con destinación económica Institucional ó cultural ó educativo ó religioso deben tener minimo una unidad de tipo Institucional y esta(s) deben ser predominantes en área construidas respecto a las demás (Aplican Excepciones en predios formales que no tienen asociada unidad de construcción pero existen unidades de construccion de predios informales).</v>
+      </c>
+      <c r="C100" s="4">
+        <v>4509</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B101" s="5" t="e">
+      <c r="A101" s="4">
+        <v>779</v>
+      </c>
+      <c r="B101" s="5" t="str">
         <f>VLOOKUP(A101,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
+        <v>total plantas de la unidad debe estar diligenciada para todas las unidades identificadas y debe ser mayor a cero (0)</v>
+      </c>
+      <c r="C101" s="4">
+        <v>89971</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add new validation rules 769 to 794 for property consistency checks
- Implement rules 769 to 794 in the SQL validation script, focusing on various conditions related to property types, including checks for 'Anexo', 'Comercial', and informal properties.
- Create corresponding tables for each rule to store validation results, detailing specific conditions that lead to non-compliance.
- Update the consolidated Excel file to reflect the new validation rules.
</commit_message>
<xml_diff>
--- a/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
+++ b/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erikka Lopez\Desktop\validaciones\IgacValidaciones\validar_consistencia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E409E5D7-81D9-4D07-B143-1064F3DAB3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CAC084-C83C-4F0A-853F-7074E244987F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="864">
   <si>
     <t>id</t>
   </si>
@@ -3100,6 +3100,15 @@
   </si>
   <si>
     <t>por el momento sin calkificaicón no puedo establecer validez de duplciados</t>
+  </si>
+  <si>
+    <t>No tenemos Dominio</t>
+  </si>
+  <si>
+    <t>No tenemos VM_ZonaHomogeneaGeoeconomicaUrbana.Valor_Metro</t>
+  </si>
+  <si>
+    <t>No tenemos VM_TipologiaConstruccion.Valor_Unitario</t>
   </si>
 </sst>
 </file>
@@ -3260,7 +3269,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3560,8 +3578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72DF236-5369-47CC-87A0-4923FC7C346E}">
   <dimension ref="A1:D236"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5041,103 +5059,154 @@
         <v>860</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B112" s="5" t="e">
+    <row r="112" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A112" s="4">
+        <v>769</v>
+      </c>
+      <c r="B112" s="5" t="str">
         <f>VLOOKUP(A112,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B113" s="5" t="e">
+        <v xml:space="preserve">Las unidades asociadas a tipos de unidades de construcción “Anexos” deben asociar solamente usos de construcción asociadas al dominio de “Anexo”   </v>
+      </c>
+      <c r="C112" s="4">
+        <v>129</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="4">
+        <v>770</v>
+      </c>
+      <c r="B113" s="5" t="str">
         <f>VLOOKUP(A113,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B114" s="5" t="e">
+        <v xml:space="preserve">Las unidades asociadas a tipos de unidades de construcción “Comercial” deben asociar solamente usos de construcción asociadas al dominio de “Comercial”   </v>
+      </c>
+      <c r="C113" s="4">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="4">
+        <v>784</v>
+      </c>
+      <c r="B114" s="5" t="str">
         <f>VLOOKUP(A114,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B115" s="5" t="e">
+        <v>Para tipo unidades de construccion residenciales, solamente se pueden asociar tipologías residenciales. (Aplican Excepciones en casos puntuales cuando a estos usos se pueden adaptar otro tipo de tipologías).</v>
+      </c>
+      <c r="C114" s="4">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="4">
+        <v>793</v>
+      </c>
+      <c r="B115" s="5" t="str">
         <f>VLOOKUP(A115,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B116" s="5" t="e">
+        <v>En la base catastral final (producto de la actualizacion catastral), si la condición del predio es Informal, entonces los campos de ILC_EstructuraAvaluo referentes a avalúo comercial terreno y avalúo catastral terreno debe ser "0".</v>
+      </c>
+      <c r="C115" s="4">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="4">
+        <v>794</v>
+      </c>
+      <c r="B116" s="5" t="str">
         <f>VLOOKUP(A116,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B117" s="5" t="e">
+        <v>En la base catastral final (producto de la actualizacion catastral), si la Destinación económica  del predio es "Lote_Urbanizable_No_Urbanizado", "Lote_Urbanizado_No_Construido", "Lote_No_Urbanizable" o "Lote_Rural", entonces los campos de ILC_EstructuraAvaluo referentes a avalúo comercial total unidades de construcción y avalúo catastral total unidades de construcción debe ser "0".</v>
+      </c>
+      <c r="C116" s="4">
+        <v>48559</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A117" s="4">
+        <v>795</v>
+      </c>
+      <c r="B117" s="5" t="str">
         <f>VLOOKUP(A117,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B118" s="5" t="e">
+        <v>El Avalúo comercial del terreno debe corresponder al resultado del producto entre el valor unitario de la zona homogénea geoeconómica ($/ha ó $/m2) y el área de terreno (ha o m2).</v>
+      </c>
+      <c r="C117" s="4">
+        <v>0</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A118" s="4">
+        <v>796</v>
+      </c>
+      <c r="B118" s="5" t="str">
         <f>VLOOKUP(A118,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+        <v>El avalúo comercial de la Unidad de Construcción debe corresponder al producto entre el valor unitario de la Tipología de construcción ($/m2) y el área construida (m2). Para los casos de Ph unidad predial y Condominio unidad predial se tendra en cuenta el área privada construida.</v>
+      </c>
+      <c r="C118" s="4">
+        <v>0</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B119" s="5" t="e">
         <f>VLOOKUP(A119,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B120" s="5" t="e">
         <f>VLOOKUP(A120,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B121" s="5" t="e">
         <f>VLOOKUP(A121,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B122" s="5" t="e">
         <f>VLOOKUP(A122,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B123" s="5" t="e">
         <f>VLOOKUP(A123,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B124" s="5" t="e">
         <f>VLOOKUP(A124,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B125" s="5" t="e">
         <f>VLOOKUP(A125,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B126" s="5" t="e">
         <f>VLOOKUP(A126,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B127" s="5" t="e">
         <f>VLOOKUP(A127,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B128" s="5" t="e">
         <f>VLOOKUP(A128,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
@@ -5798,11 +5867,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5844,7 +5914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>672</v>
       </c>
@@ -5870,7 +5940,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>681</v>
       </c>
@@ -5896,7 +5966,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>682</v>
       </c>
@@ -5922,7 +5992,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>683</v>
       </c>
@@ -5948,7 +6018,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>684</v>
       </c>
@@ -5974,7 +6044,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>685</v>
       </c>
@@ -6000,7 +6070,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>686</v>
       </c>
@@ -6026,7 +6096,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>687</v>
       </c>
@@ -6052,7 +6122,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>688</v>
       </c>
@@ -6078,7 +6148,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>689</v>
       </c>
@@ -6104,7 +6174,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="259.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>690</v>
       </c>
@@ -6130,7 +6200,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>673</v>
       </c>
@@ -6156,7 +6226,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>691</v>
       </c>
@@ -6182,7 +6252,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>692</v>
       </c>
@@ -6208,7 +6278,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="296.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="296.39999999999998" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>693</v>
       </c>
@@ -6234,7 +6304,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>694</v>
       </c>
@@ -6260,7 +6330,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>695</v>
       </c>
@@ -6286,7 +6356,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>696</v>
       </c>
@@ -6312,7 +6382,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>697</v>
       </c>
@@ -6338,7 +6408,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>698</v>
       </c>
@@ -6364,7 +6434,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>699</v>
       </c>
@@ -6390,7 +6460,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>700</v>
       </c>
@@ -6416,7 +6486,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>674</v>
       </c>
@@ -6442,7 +6512,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>701</v>
       </c>
@@ -6468,7 +6538,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>702</v>
       </c>
@@ -6494,7 +6564,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>703</v>
       </c>
@@ -6520,7 +6590,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>704</v>
       </c>
@@ -6546,7 +6616,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>705</v>
       </c>
@@ -6572,7 +6642,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>706</v>
       </c>
@@ -6598,7 +6668,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>707</v>
       </c>
@@ -6624,7 +6694,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>708</v>
       </c>
@@ -6650,7 +6720,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>709</v>
       </c>
@@ -6676,7 +6746,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>710</v>
       </c>
@@ -6702,7 +6772,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10">
         <v>675</v>
       </c>
@@ -6728,7 +6798,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>711</v>
       </c>
@@ -6754,7 +6824,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>712</v>
       </c>
@@ -6780,7 +6850,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
         <v>713</v>
       </c>
@@ -6806,7 +6876,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>714</v>
       </c>
@@ -6832,7 +6902,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>715</v>
       </c>
@@ -6858,7 +6928,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>716</v>
       </c>
@@ -6884,7 +6954,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>717</v>
       </c>
@@ -6910,7 +6980,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10">
         <v>718</v>
       </c>
@@ -6936,7 +7006,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>719</v>
       </c>
@@ -6962,7 +7032,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16">
         <v>720</v>
       </c>
@@ -6988,7 +7058,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>676</v>
       </c>
@@ -7014,7 +7084,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="73.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16">
         <v>721</v>
       </c>
@@ -7040,7 +7110,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>722</v>
       </c>
@@ -7066,7 +7136,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16">
         <v>723</v>
       </c>
@@ -7092,7 +7162,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>724</v>
       </c>
@@ -7118,7 +7188,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10">
         <v>725</v>
       </c>
@@ -7144,7 +7214,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
         <v>726</v>
       </c>
@@ -7170,7 +7240,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
         <v>727</v>
       </c>
@@ -7196,7 +7266,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
         <v>728</v>
       </c>
@@ -7222,7 +7292,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="10">
         <v>677</v>
       </c>
@@ -7248,7 +7318,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10">
         <v>678</v>
       </c>
@@ -7274,7 +7344,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10">
         <v>679</v>
       </c>
@@ -7300,7 +7370,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="10">
         <v>680</v>
       </c>
@@ -7326,7 +7396,7 @@
         <v>45815.481844355723</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="216" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="216" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10">
         <v>729</v>
       </c>
@@ -7352,7 +7422,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10">
         <v>738</v>
       </c>
@@ -7378,7 +7448,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="10">
         <v>739</v>
       </c>
@@ -7404,7 +7474,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="10">
         <v>740</v>
       </c>
@@ -7430,7 +7500,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10">
         <v>741</v>
       </c>
@@ -7456,7 +7526,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10">
         <v>742</v>
       </c>
@@ -7482,7 +7552,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10">
         <v>743</v>
       </c>
@@ -7508,7 +7578,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="10">
         <v>744</v>
       </c>
@@ -7534,7 +7604,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10">
         <v>745</v>
       </c>
@@ -7560,7 +7630,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10">
         <v>746</v>
       </c>
@@ -7586,7 +7656,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10">
         <v>747</v>
       </c>
@@ -7612,7 +7682,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10">
         <v>730</v>
       </c>
@@ -7638,7 +7708,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10">
         <v>748</v>
       </c>
@@ -7664,7 +7734,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10">
         <v>749</v>
       </c>
@@ -7690,7 +7760,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10">
         <v>750</v>
       </c>
@@ -7716,7 +7786,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10">
         <v>751</v>
       </c>
@@ -7742,7 +7812,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16">
         <v>752</v>
       </c>
@@ -7768,7 +7838,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="16">
         <v>753</v>
       </c>
@@ -7794,7 +7864,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16">
         <v>754</v>
       </c>
@@ -7820,7 +7890,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16">
         <v>755</v>
       </c>
@@ -7846,7 +7916,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="244.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16">
         <v>756</v>
       </c>
@@ -7872,7 +7942,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16">
         <v>757</v>
       </c>
@@ -7898,7 +7968,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="10">
         <v>731</v>
       </c>
@@ -7924,7 +7994,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="10">
         <v>758</v>
       </c>
@@ -7948,7 +8018,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="10">
         <v>759</v>
       </c>
@@ -7974,7 +8044,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10">
         <v>760</v>
       </c>
@@ -8000,7 +8070,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10">
         <v>761</v>
       </c>
@@ -8026,7 +8096,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="10">
         <v>732</v>
       </c>
@@ -8052,7 +8122,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="10">
         <v>733</v>
       </c>
@@ -8078,7 +8148,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="10">
         <v>734</v>
       </c>
@@ -8104,7 +8174,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="16">
         <v>735</v>
       </c>
@@ -8130,7 +8200,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="16">
         <v>736</v>
       </c>
@@ -8156,7 +8226,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="10">
         <v>737</v>
       </c>
@@ -8182,7 +8252,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10">
         <v>762</v>
       </c>
@@ -8208,7 +8278,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="20">
         <v>771</v>
       </c>
@@ -8234,7 +8304,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="20">
         <v>772</v>
       </c>
@@ -8260,7 +8330,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="20">
         <v>773</v>
       </c>
@@ -8286,7 +8356,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="10">
         <v>774</v>
       </c>
@@ -8312,7 +8382,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="10">
         <v>775</v>
       </c>
@@ -8338,7 +8408,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="10">
         <v>776</v>
       </c>
@@ -8364,7 +8434,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="10">
         <v>777</v>
       </c>
@@ -8390,7 +8460,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="10">
         <v>778</v>
       </c>
@@ -8416,7 +8486,7 @@
         <v>45815.481990740744</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="10">
         <v>779</v>
       </c>
@@ -8442,7 +8512,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="10">
         <v>780</v>
       </c>
@@ -8468,7 +8538,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="10">
         <v>763</v>
       </c>
@@ -8494,7 +8564,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="10">
         <v>781</v>
       </c>
@@ -8520,7 +8590,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="10">
         <v>782</v>
       </c>
@@ -8546,7 +8616,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="10">
         <v>783</v>
       </c>
@@ -8572,7 +8642,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="10">
         <v>764</v>
       </c>
@@ -8598,7 +8668,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16">
         <v>765</v>
       </c>
@@ -8624,7 +8694,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10">
         <v>766</v>
       </c>
@@ -8650,7 +8720,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="10">
         <v>767</v>
       </c>
@@ -8676,7 +8746,7 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="10">
         <v>768</v>
       </c>
@@ -8702,137 +8772,137 @@
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="6">
+    <row r="112" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="10">
         <v>769</v>
       </c>
-      <c r="B112" s="6" t="s">
+      <c r="B112" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C112" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D112" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="E112" s="7" t="s">
+      <c r="E112" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="F112" s="7" t="s">
+      <c r="F112" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="G112" s="7" t="s">
+      <c r="G112" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="H112" s="8">
+      <c r="H112" s="12">
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="6">
+    <row r="113" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="10">
         <v>770</v>
       </c>
-      <c r="B113" s="6" t="s">
+      <c r="B113" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="C113" s="6" t="s">
+      <c r="C113" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D113" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="E113" s="7" t="s">
+      <c r="E113" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="F113" s="7" t="s">
+      <c r="F113" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="G113" s="7" t="s">
+      <c r="G113" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="H113" s="8">
+      <c r="H113" s="12">
         <v>45815.481991131652</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="216" x14ac:dyDescent="0.3">
-      <c r="A114" s="6">
+    <row r="114" spans="1:8" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="10">
         <v>784</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="B114" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C114" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="D114" s="7" t="s">
+      <c r="D114" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="E114" s="7" t="s">
+      <c r="E114" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="F114" s="7" t="s">
+      <c r="F114" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="G114" s="7" t="s">
+      <c r="G114" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="H114" s="8">
+      <c r="H114" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A115" s="6">
+    <row r="115" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="10">
         <v>793</v>
       </c>
-      <c r="B115" s="6" t="s">
+      <c r="B115" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C115" s="6" t="s">
+      <c r="C115" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="D115" s="7" t="s">
+      <c r="D115" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="E115" s="7" t="s">
+      <c r="E115" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="F115" s="7" t="s">
+      <c r="F115" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="G115" s="7" t="s">
+      <c r="G115" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="H115" s="8">
+      <c r="H115" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="6">
+    <row r="116" spans="1:8" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="10">
         <v>794</v>
       </c>
-      <c r="B116" s="6" t="s">
+      <c r="B116" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C116" s="6" t="s">
+      <c r="C116" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="D116" s="7" t="s">
+      <c r="D116" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="E116" s="7" t="s">
+      <c r="E116" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="F116" s="7" t="s">
+      <c r="F116" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="G116" s="7" t="s">
+      <c r="G116" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="H116" s="8">
+      <c r="H116" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="16">
         <v>795</v>
       </c>
@@ -8858,29 +8928,29 @@
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A118" s="6">
+    <row r="118" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="16">
         <v>796</v>
       </c>
-      <c r="B118" s="6" t="s">
+      <c r="B118" s="16" t="s">
         <v>462</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C118" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="D118" s="7" t="s">
+      <c r="D118" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="E118" s="7" t="s">
+      <c r="E118" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="F118" s="7" t="s">
+      <c r="F118" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="G118" s="7" t="s">
+      <c r="G118" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="H118" s="8">
+      <c r="H118" s="17">
         <v>45815.482067179422</v>
       </c>
     </row>
@@ -8988,7 +9058,7 @@
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="16">
         <v>789</v>
       </c>
@@ -9115,7 +9185,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="16">
         <v>806</v>
       </c>
@@ -9137,7 +9207,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="16">
         <v>807</v>
       </c>
@@ -9159,7 +9229,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="16">
         <v>808</v>
       </c>
@@ -9181,7 +9251,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="16">
         <v>809</v>
       </c>
@@ -9203,7 +9273,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="16">
         <v>810</v>
       </c>
@@ -9225,7 +9295,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="16">
         <v>811</v>
       </c>
@@ -9247,7 +9317,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="16">
         <v>812</v>
       </c>
@@ -9378,7 +9448,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="16">
         <v>817</v>
       </c>
@@ -9400,7 +9470,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="16">
         <v>818</v>
       </c>
@@ -9422,7 +9492,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="16">
         <v>819</v>
       </c>
@@ -9444,7 +9514,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="16">
         <v>820</v>
       </c>
@@ -9466,7 +9536,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="16">
         <v>821</v>
       </c>
@@ -9488,7 +9558,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="16">
         <v>822</v>
       </c>
@@ -9510,7 +9580,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="16">
         <v>823</v>
       </c>
@@ -9532,7 +9602,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="16">
         <v>824</v>
       </c>
@@ -9554,7 +9624,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="16">
         <v>825</v>
       </c>
@@ -9576,7 +9646,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="16">
         <v>799</v>
       </c>
@@ -9598,7 +9668,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="16">
         <v>826</v>
       </c>
@@ -9663,7 +9733,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="16">
         <v>829</v>
       </c>
@@ -9685,7 +9755,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="16">
         <v>830</v>
       </c>
@@ -9707,7 +9777,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="16">
         <v>831</v>
       </c>
@@ -9729,7 +9799,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="16">
         <v>832</v>
       </c>
@@ -9751,7 +9821,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="16">
         <v>833</v>
       </c>
@@ -9773,7 +9843,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="16">
         <v>834</v>
       </c>
@@ -9795,7 +9865,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="16">
         <v>835</v>
       </c>
@@ -9817,7 +9887,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="16">
         <v>800</v>
       </c>
@@ -9839,7 +9909,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="16">
         <v>836</v>
       </c>
@@ -9861,7 +9931,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="16">
         <v>837</v>
       </c>
@@ -9883,7 +9953,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="16">
         <v>838</v>
       </c>
@@ -9905,7 +9975,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="16">
         <v>839</v>
       </c>
@@ -9927,7 +9997,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="16">
         <v>840</v>
       </c>
@@ -9969,7 +10039,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="16">
         <v>842</v>
       </c>
@@ -9993,7 +10063,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="16">
         <v>843</v>
       </c>
@@ -10017,7 +10087,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="16">
         <v>844</v>
       </c>
@@ -10041,7 +10111,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="16">
         <v>845</v>
       </c>
@@ -10065,7 +10135,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="16">
         <v>801</v>
       </c>
@@ -10110,7 +10180,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="16">
         <v>847</v>
       </c>
@@ -10134,7 +10204,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="16">
         <v>848</v>
       </c>
@@ -10198,7 +10268,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16">
         <v>851</v>
       </c>
@@ -10220,7 +10290,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16">
         <v>852</v>
       </c>
@@ -10242,7 +10312,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16">
         <v>802</v>
       </c>
@@ -10264,7 +10334,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16">
         <v>803</v>
       </c>
@@ -10286,7 +10356,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16">
         <v>804</v>
       </c>
@@ -10308,7 +10378,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16">
         <v>805</v>
       </c>
@@ -10350,7 +10420,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="16">
         <v>862</v>
       </c>
@@ -10374,7 +10444,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16">
         <v>863</v>
       </c>
@@ -10398,7 +10468,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16">
         <v>864</v>
       </c>
@@ -10511,7 +10581,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16">
         <v>854</v>
       </c>
@@ -10535,7 +10605,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16">
         <v>855</v>
       </c>
@@ -10559,7 +10629,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16">
         <v>856</v>
       </c>
@@ -10583,7 +10653,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16">
         <v>857</v>
       </c>
@@ -10607,7 +10677,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16">
         <v>858</v>
       </c>
@@ -10631,7 +10701,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16">
         <v>859</v>
       </c>
@@ -10655,7 +10725,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16">
         <v>860</v>
       </c>
@@ -10679,7 +10749,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16">
         <v>861</v>
       </c>
@@ -10703,7 +10773,7 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="16">
         <v>869</v>
       </c>
@@ -10755,7 +10825,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="16">
         <v>879</v>
       </c>
@@ -10781,7 +10851,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="16">
         <v>880</v>
       </c>
@@ -10807,7 +10877,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="16">
         <v>881</v>
       </c>
@@ -10833,7 +10903,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="16">
         <v>882</v>
       </c>
@@ -10859,7 +10929,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" ht="302.39999999999998" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="16">
         <v>883</v>
       </c>
@@ -10885,7 +10955,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" ht="316.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="16">
         <v>884</v>
       </c>
@@ -10911,7 +10981,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" ht="273.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="16">
         <v>885</v>
       </c>
@@ -10937,7 +11007,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="288" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" ht="288" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="16">
         <v>886</v>
       </c>
@@ -10963,7 +11033,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6">
         <v>887</v>
       </c>
@@ -10989,7 +11059,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6">
         <v>870</v>
       </c>
@@ -11015,7 +11085,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="6">
         <v>888</v>
       </c>
@@ -11041,7 +11111,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="6">
         <v>889</v>
       </c>
@@ -11067,7 +11137,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="6">
         <v>890</v>
       </c>
@@ -11093,7 +11163,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="214" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="6">
         <v>891</v>
       </c>
@@ -11119,7 +11189,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="6">
         <v>892</v>
       </c>
@@ -11145,7 +11215,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="6">
         <v>893</v>
       </c>
@@ -11171,7 +11241,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="217" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6">
         <v>894</v>
       </c>
@@ -11197,7 +11267,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="6">
         <v>895</v>
       </c>
@@ -11223,7 +11293,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="219" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6">
         <v>871</v>
       </c>
@@ -11249,7 +11319,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="6">
         <v>872</v>
       </c>
@@ -11275,7 +11345,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6">
         <v>873</v>
       </c>
@@ -11301,7 +11371,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="6">
         <v>874</v>
       </c>
@@ -11327,7 +11397,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6">
         <v>875</v>
       </c>
@@ -11353,7 +11423,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6">
         <v>876</v>
       </c>
@@ -11379,7 +11449,7 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" ht="273.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="6">
         <v>877</v>
       </c>
@@ -11406,7 +11476,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H225" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H225" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new validation rules 785 to 792 for property consistency checks
- Implement rules 785 to 792 in the SQL validation script, focusing on various conditions related to property types, including checks for 'Comercial', 'Industrial', 'Institucional', and 'Anexo'.
- Create corresponding tables for each rule to store validation results, detailing specific conditions that lead to non-compliance.
- Update the consolidated Excel file to reflect the new validation rules.
</commit_message>
<xml_diff>
--- a/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
+++ b/validar_consistencia/data/listado_consolidado_consistencia_reglas.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erikka Lopez\Desktop\validaciones\IgacValidaciones\validar_consistencia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CAC084-C83C-4F0A-853F-7074E244987F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31D57CC-F153-4D4F-A0DF-F9B3F07A17A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$236</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$H$225</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="867">
   <si>
     <t>id</t>
   </si>
@@ -3109,6 +3110,15 @@
   </si>
   <si>
     <t>No tenemos VM_TipologiaConstruccion.Valor_Unitario</t>
+  </si>
+  <si>
+    <t>7/06/2025  11:34:11 a. m.+A119:H119</t>
+  </si>
+  <si>
+    <t>7/06/2025  11:34:11 a. m.+A120:H120</t>
+  </si>
+  <si>
+    <t>No tenemos esos datos</t>
   </si>
 </sst>
 </file>
@@ -3132,7 +3142,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3169,6 +3179,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3197,7 +3231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3265,20 +3299,53 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3576,10 +3643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72DF236-5369-47CC-87A0-4923FC7C346E}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D236"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3602,7 +3670,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>672</v>
       </c>
@@ -3616,7 +3684,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>672</v>
       </c>
@@ -3630,7 +3698,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>672</v>
       </c>
@@ -3644,7 +3712,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>672</v>
       </c>
@@ -3658,7 +3726,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>672</v>
       </c>
@@ -3686,7 +3754,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>681</v>
       </c>
@@ -3700,7 +3768,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>685</v>
       </c>
@@ -3711,7 +3779,7 @@
         <v>288085</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>686</v>
       </c>
@@ -3722,7 +3790,7 @@
         <v>140151</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>688</v>
       </c>
@@ -3733,7 +3801,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>689</v>
       </c>
@@ -3744,7 +3812,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>690</v>
       </c>
@@ -3758,7 +3826,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>673</v>
       </c>
@@ -3772,7 +3840,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>692</v>
       </c>
@@ -3786,7 +3854,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="273.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>693</v>
       </c>
@@ -3800,7 +3868,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>694</v>
       </c>
@@ -3814,7 +3882,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>695</v>
       </c>
@@ -3828,7 +3896,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>696</v>
       </c>
@@ -3842,7 +3910,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>697</v>
       </c>
@@ -3856,7 +3924,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>698</v>
       </c>
@@ -3870,7 +3938,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>699</v>
       </c>
@@ -3884,7 +3952,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>700</v>
       </c>
@@ -3898,18 +3966,18 @@
         <v>839</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+    <row r="24" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="35">
         <v>674</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="35">
         <v>6553</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>701</v>
       </c>
@@ -3923,7 +3991,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>702</v>
       </c>
@@ -3937,7 +4005,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>703</v>
       </c>
@@ -3951,7 +4019,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>704</v>
       </c>
@@ -3965,7 +4033,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>705</v>
       </c>
@@ -3979,7 +4047,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>706</v>
       </c>
@@ -3993,7 +4061,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>707</v>
       </c>
@@ -4007,7 +4075,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>708</v>
       </c>
@@ -4021,7 +4089,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>709</v>
       </c>
@@ -4035,7 +4103,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>710</v>
       </c>
@@ -4049,7 +4117,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>675</v>
       </c>
@@ -4063,7 +4131,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>711</v>
       </c>
@@ -4077,7 +4145,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>712</v>
       </c>
@@ -4091,7 +4159,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>713</v>
       </c>
@@ -4102,7 +4170,7 @@
         <v>3393</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>714</v>
       </c>
@@ -4116,7 +4184,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>715</v>
       </c>
@@ -4130,7 +4198,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>716</v>
       </c>
@@ -4141,7 +4209,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>717</v>
       </c>
@@ -4152,7 +4220,7 @@
         <v>254827</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>718</v>
       </c>
@@ -4166,7 +4234,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>719</v>
       </c>
@@ -4180,7 +4248,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>720</v>
       </c>
@@ -4194,7 +4262,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18">
         <v>676</v>
       </c>
@@ -4208,7 +4276,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>721</v>
       </c>
@@ -4222,7 +4290,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>722</v>
       </c>
@@ -4236,7 +4304,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>723</v>
       </c>
@@ -4250,7 +4318,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>724</v>
       </c>
@@ -4264,7 +4332,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>725</v>
       </c>
@@ -4278,7 +4346,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>726</v>
       </c>
@@ -4292,7 +4360,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>727</v>
       </c>
@@ -4306,7 +4374,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>728</v>
       </c>
@@ -4320,18 +4388,19 @@
         <v>848</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
+    <row r="55" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="35">
         <v>677</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="35">
         <v>27577</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D55" s="36"/>
+    </row>
+    <row r="56" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>678</v>
       </c>
@@ -4345,7 +4414,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>679</v>
       </c>
@@ -4359,18 +4428,19 @@
         <v>841</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4">
+    <row r="58" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="35">
         <v>680</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="35">
         <v>37</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="D58" s="36"/>
+    </row>
+    <row r="59" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>729</v>
       </c>
@@ -4384,7 +4454,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>738</v>
       </c>
@@ -4398,7 +4468,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>739</v>
       </c>
@@ -4412,7 +4482,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>740</v>
       </c>
@@ -4426,7 +4496,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>741</v>
       </c>
@@ -4440,7 +4510,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>742</v>
       </c>
@@ -4451,7 +4521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>743</v>
       </c>
@@ -4462,7 +4532,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>744</v>
       </c>
@@ -4474,7 +4544,7 @@
         <v>6128</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>745</v>
       </c>
@@ -4486,7 +4556,7 @@
         <v>60361</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>746</v>
       </c>
@@ -4498,7 +4568,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>747</v>
       </c>
@@ -4510,7 +4580,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>730</v>
       </c>
@@ -4522,7 +4592,7 @@
         <v>58813</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>748</v>
       </c>
@@ -4534,7 +4604,7 @@
         <v>23394</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>749</v>
       </c>
@@ -4546,7 +4616,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>750</v>
       </c>
@@ -4558,7 +4628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>751</v>
       </c>
@@ -4570,7 +4640,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>752</v>
       </c>
@@ -4585,7 +4655,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>753</v>
       </c>
@@ -4600,7 +4670,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>754</v>
       </c>
@@ -4615,7 +4685,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>755</v>
       </c>
@@ -4630,7 +4700,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>756</v>
       </c>
@@ -4645,7 +4715,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>757</v>
       </c>
@@ -4660,7 +4730,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>731</v>
       </c>
@@ -4672,7 +4742,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>758</v>
       </c>
@@ -4687,7 +4757,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>759</v>
       </c>
@@ -4699,7 +4769,7 @@
         <v>25711</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>760</v>
       </c>
@@ -4711,7 +4781,7 @@
         <v>25711</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>761</v>
       </c>
@@ -4726,7 +4796,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>732</v>
       </c>
@@ -4738,7 +4808,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>733</v>
       </c>
@@ -4750,7 +4820,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>734</v>
       </c>
@@ -4762,7 +4832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>735</v>
       </c>
@@ -4777,7 +4847,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>736</v>
       </c>
@@ -4792,7 +4862,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>737</v>
       </c>
@@ -4804,7 +4874,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>762</v>
       </c>
@@ -4816,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>771</v>
       </c>
@@ -4831,7 +4901,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>772</v>
       </c>
@@ -4846,7 +4916,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>773</v>
       </c>
@@ -4861,7 +4931,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>774</v>
       </c>
@@ -4873,7 +4943,7 @@
         <v>318213</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>775</v>
       </c>
@@ -4885,7 +4955,7 @@
         <v>115299</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>776</v>
       </c>
@@ -4897,7 +4967,7 @@
         <v>2705</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>777</v>
       </c>
@@ -4909,7 +4979,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>778</v>
       </c>
@@ -4921,7 +4991,7 @@
         <v>4509</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>779</v>
       </c>
@@ -4933,7 +5003,7 @@
         <v>89971</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>780</v>
       </c>
@@ -4945,7 +5015,7 @@
         <v>53375</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>763</v>
       </c>
@@ -4957,7 +5027,7 @@
         <v>10247</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>781</v>
       </c>
@@ -4969,7 +5039,7 @@
         <v>57024</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>782</v>
       </c>
@@ -4981,7 +5051,7 @@
         <v>114436</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>783</v>
       </c>
@@ -4993,7 +5063,7 @@
         <v>204704</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>764</v>
       </c>
@@ -5005,7 +5075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>765</v>
       </c>
@@ -5020,7 +5090,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>766</v>
       </c>
@@ -5032,7 +5102,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>767</v>
       </c>
@@ -5044,7 +5114,7 @@
         <v>116765</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>768</v>
       </c>
@@ -5059,7 +5129,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>769</v>
       </c>
@@ -5074,7 +5144,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
         <v>770</v>
       </c>
@@ -5086,7 +5156,7 @@
         <v>4460</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>784</v>
       </c>
@@ -5098,7 +5168,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>793</v>
       </c>
@@ -5110,7 +5180,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
         <v>794</v>
       </c>
@@ -5122,7 +5192,7 @@
         <v>48559</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
         <v>795</v>
       </c>
@@ -5137,7 +5207,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>796</v>
       </c>
@@ -5152,715 +5222,782 @@
         <v>863</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B119" s="5" t="e">
+    <row r="119" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="4">
+        <v>785</v>
+      </c>
+      <c r="B119" s="5" t="str">
         <f>VLOOKUP(A119,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B120" s="5" t="e">
+        <v>Para tipo unidades de construccion comerciales, solamente se pueden asociar tipologías comerciales. (Aplican Excepciones en casos puntuales cuando a estos usos se pueden adaptar otro tipo de tipologías).</v>
+      </c>
+      <c r="C119" s="4">
+        <v>6555</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="4">
+        <v>786</v>
+      </c>
+      <c r="B120" s="5" t="str">
         <f>VLOOKUP(A120,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B121" s="5" t="e">
+        <v>Paratipo unidades de construccion  industriales,, solamente se pueden asociar tipologías industriales. (Aplican Excepciones en casos puntuales cuando a estos usos se pueden adaptar otro tipo de tipologías).</v>
+      </c>
+      <c r="C120" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="4">
+        <v>787</v>
+      </c>
+      <c r="B121" s="5" t="str">
         <f>VLOOKUP(A121,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B122" s="5" t="e">
+        <v>Para tipo unidades de construccion institucionales, solamente se pueden asociar tipologías institucionales. (Aplican Excepciones en casos puntuales cuando a estos usos se pueden adaptar otro tipo de tipologías).</v>
+      </c>
+      <c r="C121" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="4">
+        <v>788</v>
+      </c>
+      <c r="B122" s="5" t="str">
         <f>VLOOKUP(A122,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B123" s="5" t="e">
+        <v>Para tipo unidades de construccion Anexos, solamente se pueden asociar tipo Anexos. (Aplican Excepciones en casos puntuales cuando a estos usos se pueden adaptar otro tipo de tipologías).</v>
+      </c>
+      <c r="C122" s="4">
+        <v>43291</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="4">
+        <v>789</v>
+      </c>
+      <c r="B123" s="5" t="str">
         <f>VLOOKUP(A123,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B124" s="5" t="e">
+        <v>En la base catastral final (producto de la actualizacion catastral) se debe registrar el avalúo del predio exceptuando los predios cancelados</v>
+      </c>
+      <c r="C123" s="4">
+        <v>0</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="4">
+        <v>790</v>
+      </c>
+      <c r="B124" s="5" t="str">
         <f>VLOOKUP(A124,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B125" s="5" t="e">
+        <v>En la base catastral final (producto de la actualizacion catastral) el avaluo comercial registrado debe corresponder a la sumatoria del avalúo comercial de terreno mas el avaluo comercial total de las unidades de construcción y este valor debe se mayor a "0".</v>
+      </c>
+      <c r="C124" s="4">
+        <v>638857</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="4">
+        <v>791</v>
+      </c>
+      <c r="B125" s="5" t="str">
         <f>VLOOKUP(A125,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B126" s="5" t="e">
+        <v>En la base catastral final (producto de la actualizacion catastral) el avaluo catastral registrado debe corresponder a la sumatoria del avalúo catastral de terreno mas el avaluo catastral total de las unidade de construcción  y este valor debe se mayor a "0".</v>
+      </c>
+      <c r="C125" s="4">
+        <v>638857</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="4">
+        <v>792</v>
+      </c>
+      <c r="B126" s="5" t="str">
         <f>VLOOKUP(A126,Sheet1!A:D,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+        <v>En la base catastral final (producto de la actualizacion catastral) los campos de ILC_EstructuraAvaluo referentes a avalúo catastral, deben ser mayor al 60% y menor que el 100%  del avalúo comercial y este valor debe ser mayor a "0".</v>
+      </c>
+      <c r="C126" s="4">
+        <v>638857</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="B127" s="5" t="e">
         <f>VLOOKUP(A127,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="B128" s="5" t="e">
         <f>VLOOKUP(A128,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="e">
         <f>VLOOKUP(A129,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B130" s="5" t="e">
         <f>VLOOKUP(A130,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B131" s="5" t="e">
         <f>VLOOKUP(A131,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B132" s="5" t="e">
         <f>VLOOKUP(A132,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B133" s="5" t="e">
         <f>VLOOKUP(A133,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B134" s="5" t="e">
         <f>VLOOKUP(A134,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B135" s="5" t="e">
         <f>VLOOKUP(A135,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B136" s="5" t="e">
         <f>VLOOKUP(A136,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B137" s="5" t="e">
         <f>VLOOKUP(A137,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B138" s="5" t="e">
         <f>VLOOKUP(A138,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B139" s="5" t="e">
         <f>VLOOKUP(A139,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B140" s="5" t="e">
         <f>VLOOKUP(A140,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B141" s="5" t="e">
         <f>VLOOKUP(A141,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B142" s="5" t="e">
         <f>VLOOKUP(A142,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B143" s="5" t="e">
         <f>VLOOKUP(A143,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B144" s="5" t="e">
         <f>VLOOKUP(A144,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B145" s="5" t="e">
         <f>VLOOKUP(A145,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B146" s="5" t="e">
         <f>VLOOKUP(A146,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B147" s="5" t="e">
         <f>VLOOKUP(A147,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B148" s="5" t="e">
         <f>VLOOKUP(A148,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B149" s="5" t="e">
         <f>VLOOKUP(A149,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B150" s="5" t="e">
         <f>VLOOKUP(A150,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B151" s="5" t="e">
         <f>VLOOKUP(A151,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B152" s="5" t="e">
         <f>VLOOKUP(A152,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B153" s="5" t="e">
         <f>VLOOKUP(A153,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B154" s="5" t="e">
         <f>VLOOKUP(A154,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B155" s="5" t="e">
         <f>VLOOKUP(A155,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B156" s="5" t="e">
         <f>VLOOKUP(A156,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B157" s="5" t="e">
         <f>VLOOKUP(A157,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B158" s="5" t="e">
         <f>VLOOKUP(A158,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B159" s="5" t="e">
         <f>VLOOKUP(A159,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B160" s="5" t="e">
         <f>VLOOKUP(A160,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B161" s="5" t="e">
         <f>VLOOKUP(A161,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B162" s="5" t="e">
         <f>VLOOKUP(A162,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B163" s="5" t="e">
         <f>VLOOKUP(A163,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B164" s="5" t="e">
         <f>VLOOKUP(A164,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B165" s="5" t="e">
         <f>VLOOKUP(A165,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B166" s="5" t="e">
         <f>VLOOKUP(A166,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B167" s="5" t="e">
         <f>VLOOKUP(A167,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B168" s="5" t="e">
         <f>VLOOKUP(A168,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B169" s="5" t="e">
         <f>VLOOKUP(A169,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B170" s="5" t="e">
         <f>VLOOKUP(A170,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B171" s="5" t="e">
         <f>VLOOKUP(A171,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B172" s="5" t="e">
         <f>VLOOKUP(A172,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B173" s="5" t="e">
         <f>VLOOKUP(A173,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B174" s="5" t="e">
         <f>VLOOKUP(A174,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B175" s="5" t="e">
         <f>VLOOKUP(A175,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B176" s="5" t="e">
         <f>VLOOKUP(A176,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B177" s="5" t="e">
         <f>VLOOKUP(A177,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B178" s="5" t="e">
         <f>VLOOKUP(A178,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B179" s="5" t="e">
         <f>VLOOKUP(A179,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B180" s="5" t="e">
         <f>VLOOKUP(A180,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B181" s="5" t="e">
         <f>VLOOKUP(A181,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B182" s="5" t="e">
         <f>VLOOKUP(A182,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B183" s="5" t="e">
         <f>VLOOKUP(A183,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B184" s="5" t="e">
         <f>VLOOKUP(A184,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B185" s="5" t="e">
         <f>VLOOKUP(A185,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B186" s="5" t="e">
         <f>VLOOKUP(A186,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B187" s="5" t="e">
         <f>VLOOKUP(A187,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B188" s="5" t="e">
         <f>VLOOKUP(A188,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B189" s="5" t="e">
         <f>VLOOKUP(A189,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B190" s="5" t="e">
         <f>VLOOKUP(A190,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B191" s="5" t="e">
         <f>VLOOKUP(A191,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B192" s="5" t="e">
         <f>VLOOKUP(A192,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B193" s="5" t="e">
         <f>VLOOKUP(A193,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B194" s="5" t="e">
         <f>VLOOKUP(A194,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B195" s="5" t="e">
         <f>VLOOKUP(A195,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B196" s="5" t="e">
         <f>VLOOKUP(A196,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B197" s="5" t="e">
         <f>VLOOKUP(A197,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B198" s="5" t="e">
         <f>VLOOKUP(A198,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B199" s="5" t="e">
         <f>VLOOKUP(A199,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B200" s="5" t="e">
         <f>VLOOKUP(A200,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B201" s="5" t="e">
         <f>VLOOKUP(A201,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B202" s="5" t="e">
         <f>VLOOKUP(A202,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B203" s="5" t="e">
         <f>VLOOKUP(A203,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B204" s="5" t="e">
         <f>VLOOKUP(A204,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B205" s="5" t="e">
         <f>VLOOKUP(A205,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B206" s="5" t="e">
         <f>VLOOKUP(A206,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B207" s="5" t="e">
         <f>VLOOKUP(A207,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B208" s="5" t="e">
         <f>VLOOKUP(A208,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B209" s="5" t="e">
         <f>VLOOKUP(A209,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B210" s="5" t="e">
         <f>VLOOKUP(A210,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B211" s="5" t="e">
         <f>VLOOKUP(A211,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B212" s="5" t="e">
         <f>VLOOKUP(A212,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B213" s="5" t="e">
         <f>VLOOKUP(A213,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B214" s="5" t="e">
         <f>VLOOKUP(A214,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B215" s="5" t="e">
         <f>VLOOKUP(A215,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B216" s="5" t="e">
         <f>VLOOKUP(A216,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B217" s="5" t="e">
         <f>VLOOKUP(A217,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B218" s="5" t="e">
         <f>VLOOKUP(A218,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B219" s="5" t="e">
         <f>VLOOKUP(A219,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B220" s="5" t="e">
         <f>VLOOKUP(A220,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B221" s="5" t="e">
         <f>VLOOKUP(A221,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B222" s="5" t="e">
         <f>VLOOKUP(A222,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B223" s="5" t="e">
         <f>VLOOKUP(A223,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B224" s="5" t="e">
         <f>VLOOKUP(A224,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B225" s="5" t="e">
         <f>VLOOKUP(A225,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B226" s="5" t="e">
         <f>VLOOKUP(A226,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B227" s="5" t="e">
         <f>VLOOKUP(A227,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B228" s="5" t="e">
         <f>VLOOKUP(A228,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B229" s="5" t="e">
         <f>VLOOKUP(A229,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B230" s="5" t="e">
         <f>VLOOKUP(A230,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B231" s="5" t="e">
         <f>VLOOKUP(A231,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B232" s="5" t="e">
         <f>VLOOKUP(A232,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B233" s="5" t="e">
         <f>VLOOKUP(A233,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B234" s="5" t="e">
         <f>VLOOKUP(A234,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B235" s="5" t="e">
         <f>VLOOKUP(A235,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B236" s="5" t="e">
         <f>VLOOKUP(A236,Sheet1!A:D,4,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B236" xr:uid="{D72DF236-5369-47CC-87A0-4923FC7C346E}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="691"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5870,9 +6007,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G119" sqref="G119"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D231" sqref="D231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8018,7 +8155,7 @@
         <v>45815.481918296238</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="10">
         <v>759</v>
       </c>
@@ -8954,107 +9091,107 @@
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A119" s="6">
+    <row r="119" spans="1:8" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="10">
         <v>785</v>
       </c>
-      <c r="B119" s="6" t="s">
+      <c r="B119" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C119" s="6" t="s">
+      <c r="C119" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="D119" s="7" t="s">
+      <c r="D119" s="11" t="s">
         <v>488</v>
       </c>
-      <c r="E119" s="7" t="s">
+      <c r="E119" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="F119" s="7" t="s">
+      <c r="F119" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="G119" s="7" t="s">
+      <c r="G119" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="H119" s="8">
+      <c r="H119" s="12" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="10">
+        <v>786</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="G120" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="H120" s="12" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="10">
+        <v>787</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="H121" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="6">
-        <v>786</v>
-      </c>
-      <c r="B120" s="6" t="s">
+    <row r="122" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="10">
+        <v>788</v>
+      </c>
+      <c r="B122" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C120" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="E120" s="7" t="s">
+      <c r="C122" s="10" t="s">
+        <v>496</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="E122" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="F120" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="G120" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="H120" s="8">
-        <v>45815.482067179422</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="6">
-        <v>787</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>494</v>
-      </c>
-      <c r="E121" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="F121" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="G121" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="H121" s="8">
-        <v>45815.482067179422</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="6">
-        <v>788</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>497</v>
-      </c>
-      <c r="E122" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="F122" s="7" t="s">
+      <c r="F122" s="11" t="s">
         <v>498</v>
       </c>
-      <c r="G122" s="7" t="s">
+      <c r="G122" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="H122" s="8">
+      <c r="H122" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
@@ -9084,104 +9221,105 @@
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A124" s="6">
+    <row r="124" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="10">
         <v>790</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B124" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C124" s="6" t="s">
+      <c r="C124" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D124" s="11" t="s">
         <v>506</v>
       </c>
-      <c r="E124" s="7" t="s">
+      <c r="E124" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="F124" s="7" t="s">
+      <c r="F124" s="11" t="s">
         <v>507</v>
       </c>
-      <c r="G124" s="7" t="s">
+      <c r="G124" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="H124" s="8">
+      <c r="H124" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A125" s="6">
+    <row r="125" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="10">
         <v>791</v>
       </c>
-      <c r="B125" s="6" t="s">
+      <c r="B125" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C125" s="6" t="s">
+      <c r="C125" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="D125" s="7" t="s">
+      <c r="D125" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="E125" s="7" t="s">
+      <c r="E125" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="F125" s="7" t="s">
+      <c r="F125" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="G125" s="7" t="s">
+      <c r="G125" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="H125" s="8">
+      <c r="H125" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A126" s="6">
+    <row r="126" spans="1:8" ht="331.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="10">
         <v>792</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="B126" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C126" s="6" t="s">
+      <c r="C126" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="D126" s="7" t="s">
+      <c r="D126" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="E126" s="7" t="s">
+      <c r="E126" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="F126" s="7" t="s">
+      <c r="F126" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="G126" s="7" t="s">
+      <c r="G126" s="11" t="s">
         <v>515</v>
       </c>
-      <c r="H126" s="8">
+      <c r="H126" s="12">
         <v>45815.482067179422</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A127" s="6">
+    <row r="127" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="23">
         <v>797</v>
       </c>
-      <c r="B127" s="6" t="s">
+      <c r="B127" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="C127" s="6" t="s">
+      <c r="C127" s="23" t="s">
         <v>517</v>
       </c>
-      <c r="D127" s="7" t="s">
+      <c r="D127" s="24" t="s">
         <v>518</v>
       </c>
-      <c r="E127" s="7" t="s">
+      <c r="E127" s="24" t="s">
         <v>519</v>
       </c>
-      <c r="F127" s="7" t="s">
+      <c r="F127" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H127" s="8">
+      <c r="G127" s="24"/>
+      <c r="H127" s="25">
         <v>45815.482136612532</v>
       </c>
     </row>
@@ -9339,112 +9477,119 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A135" s="6">
+    <row r="135" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="23">
         <v>813</v>
       </c>
-      <c r="B135" s="6" t="s">
+      <c r="B135" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="C135" s="6" t="s">
+      <c r="C135" s="23" t="s">
         <v>541</v>
       </c>
-      <c r="D135" s="7" t="s">
+      <c r="D135" s="24" t="s">
         <v>542</v>
       </c>
-      <c r="E135" s="7" t="s">
+      <c r="E135" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="H135" s="8">
+      <c r="F135" s="24"/>
+      <c r="G135" s="24"/>
+      <c r="H135" s="25">
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A136" s="6">
+    <row r="136" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="23">
         <v>814</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B136" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C136" s="23" t="s">
         <v>544</v>
       </c>
-      <c r="D136" s="7" t="s">
+      <c r="D136" s="24" t="s">
         <v>545</v>
       </c>
-      <c r="E136" s="7" t="s">
+      <c r="E136" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="H136" s="8">
+      <c r="F136" s="24"/>
+      <c r="G136" s="24"/>
+      <c r="H136" s="25">
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="6">
+    <row r="137" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="23">
         <v>815</v>
       </c>
-      <c r="B137" s="6" t="s">
+      <c r="B137" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="C137" s="6" t="s">
+      <c r="C137" s="23" t="s">
         <v>546</v>
       </c>
-      <c r="D137" s="7" t="s">
+      <c r="D137" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="E137" s="7" t="s">
+      <c r="E137" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="F137" s="7" t="s">
+      <c r="F137" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="H137" s="8">
+      <c r="G137" s="24"/>
+      <c r="H137" s="25">
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A138" s="6">
+    <row r="138" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="23">
         <v>798</v>
       </c>
-      <c r="B138" s="6" t="s">
+      <c r="B138" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="C138" s="6" t="s">
+      <c r="C138" s="23" t="s">
         <v>550</v>
       </c>
-      <c r="D138" s="7" t="s">
+      <c r="D138" s="24" t="s">
         <v>551</v>
       </c>
-      <c r="E138" s="7" t="s">
+      <c r="E138" s="24" t="s">
         <v>519</v>
       </c>
-      <c r="F138" s="7" t="s">
+      <c r="F138" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H138" s="8">
+      <c r="G138" s="24"/>
+      <c r="H138" s="25">
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="6">
+    <row r="139" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="23">
         <v>816</v>
       </c>
-      <c r="B139" s="6" t="s">
+      <c r="B139" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="C139" s="6" t="s">
+      <c r="C139" s="23" t="s">
         <v>552</v>
       </c>
-      <c r="D139" s="7" t="s">
+      <c r="D139" s="24" t="s">
         <v>553</v>
       </c>
-      <c r="E139" s="7" t="s">
+      <c r="E139" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="F139" s="7" t="s">
+      <c r="F139" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="H139" s="8">
+      <c r="G139" s="24"/>
+      <c r="H139" s="25">
         <v>45815.482136612532</v>
       </c>
     </row>
@@ -9690,46 +9835,49 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A151" s="6">
+    <row r="151" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="26">
         <v>827</v>
       </c>
-      <c r="B151" s="6" t="s">
+      <c r="B151" s="26" t="s">
         <v>516</v>
       </c>
-      <c r="C151" s="6" t="s">
+      <c r="C151" s="26" t="s">
         <v>583</v>
       </c>
-      <c r="D151" s="7" t="s">
+      <c r="D151" s="27" t="s">
         <v>584</v>
       </c>
-      <c r="E151" s="7" t="s">
+      <c r="E151" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="F151" s="7" t="s">
+      <c r="F151" s="27" t="s">
         <v>585</v>
       </c>
-      <c r="H151" s="8">
+      <c r="G151" s="27"/>
+      <c r="H151" s="28">
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="6">
+    <row r="152" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="26">
         <v>828</v>
       </c>
-      <c r="B152" s="6" t="s">
+      <c r="B152" s="26" t="s">
         <v>516</v>
       </c>
-      <c r="C152" s="6" t="s">
+      <c r="C152" s="26" t="s">
         <v>586</v>
       </c>
-      <c r="D152" s="7" t="s">
+      <c r="D152" s="27" t="s">
         <v>587</v>
       </c>
-      <c r="E152" s="7" t="s">
+      <c r="E152" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="H152" s="8">
+      <c r="F152" s="27"/>
+      <c r="G152" s="27"/>
+      <c r="H152" s="28">
         <v>45815.482136612532</v>
       </c>
     </row>
@@ -10019,7 +10167,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
         <v>841</v>
       </c>
@@ -10157,7 +10305,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
         <v>846</v>
       </c>
@@ -10228,7 +10376,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
         <v>849</v>
       </c>
@@ -10248,7 +10396,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6">
         <v>850</v>
       </c>
@@ -10400,7 +10548,7 @@
         <v>45815.482136612532</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6">
         <v>853</v>
       </c>
@@ -10492,92 +10640,97 @@
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A187" s="6">
+    <row r="187" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="32">
         <v>865</v>
       </c>
-      <c r="B187" s="6" t="s">
+      <c r="B187" s="32" t="s">
         <v>666</v>
       </c>
-      <c r="C187" s="6" t="s">
+      <c r="C187" s="32" t="s">
         <v>680</v>
       </c>
-      <c r="D187" s="7" t="s">
+      <c r="D187" s="33" t="s">
         <v>681</v>
       </c>
-      <c r="E187" s="7" t="s">
+      <c r="E187" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F187" s="7" t="s">
+      <c r="F187" s="33" t="s">
         <v>682</v>
       </c>
-      <c r="H187" s="8">
+      <c r="G187" s="33"/>
+      <c r="H187" s="34">
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A188" s="6">
+    <row r="188" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="32">
         <v>866</v>
       </c>
-      <c r="B188" s="6" t="s">
+      <c r="B188" s="32" t="s">
         <v>666</v>
       </c>
-      <c r="C188" s="6" t="s">
+      <c r="C188" s="32" t="s">
         <v>683</v>
       </c>
-      <c r="D188" s="7" t="s">
+      <c r="D188" s="33" t="s">
         <v>684</v>
       </c>
-      <c r="E188" s="7" t="s">
+      <c r="E188" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F188" s="7" t="s">
+      <c r="F188" s="33" t="s">
         <v>685</v>
       </c>
-      <c r="H188" s="8">
+      <c r="G188" s="33"/>
+      <c r="H188" s="34">
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A189" s="6">
+    <row r="189" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="32">
         <v>867</v>
       </c>
-      <c r="B189" s="6" t="s">
+      <c r="B189" s="32" t="s">
         <v>666</v>
       </c>
-      <c r="C189" s="6" t="s">
+      <c r="C189" s="32" t="s">
         <v>686</v>
       </c>
-      <c r="D189" s="7" t="s">
+      <c r="D189" s="33" t="s">
         <v>687</v>
       </c>
-      <c r="E189" s="7" t="s">
+      <c r="E189" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F189" s="7" t="s">
+      <c r="F189" s="33" t="s">
         <v>688</v>
       </c>
-      <c r="H189" s="8">
+      <c r="G189" s="33"/>
+      <c r="H189" s="34">
         <v>45815.482208482339</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A190" s="6">
+    <row r="190" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="29">
         <v>868</v>
       </c>
-      <c r="B190" s="6" t="s">
+      <c r="B190" s="29" t="s">
         <v>666</v>
       </c>
-      <c r="C190" s="6" t="s">
+      <c r="C190" s="29" t="s">
         <v>689</v>
       </c>
-      <c r="D190" s="7" t="s">
+      <c r="D190" s="30" t="s">
         <v>690</v>
       </c>
-      <c r="E190" s="7" t="s">
+      <c r="E190" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="H190" s="8">
+      <c r="F190" s="30"/>
+      <c r="G190" s="30"/>
+      <c r="H190" s="31">
         <v>45815.482208482339</v>
       </c>
     </row>
@@ -10799,29 +10952,29 @@
         <v>45815.482283591147</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A200" s="6">
+    <row r="200" spans="1:8" ht="244.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="16">
         <v>878</v>
       </c>
-      <c r="B200" s="6" t="s">
+      <c r="B200" s="16" t="s">
         <v>719</v>
       </c>
-      <c r="C200" s="6" t="s">
+      <c r="C200" s="16" t="s">
         <v>725</v>
       </c>
-      <c r="D200" s="7" t="s">
+      <c r="D200" s="9" t="s">
         <v>726</v>
       </c>
-      <c r="E200" s="7" t="s">
+      <c r="E200" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F200" s="7" t="s">
+      <c r="F200" s="9" t="s">
         <v>727</v>
       </c>
-      <c r="G200" s="7" t="s">
+      <c r="G200" s="9" t="s">
         <v>728</v>
       </c>
-      <c r="H200" s="8">
+      <c r="H200" s="17">
         <v>45815.482283591147</v>
       </c>
     </row>
@@ -11477,8 +11630,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H225" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <colorFilter dxfId="0"/>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="759"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>